<commit_message>
fixed portPosX, updated specs, rezie childs prototype
</commit_message>
<xml_diff>
--- a/specs/ClassHirachieAndPersistentAttributes.xlsx
+++ b/specs/ClassHirachieAndPersistentAttributes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Draw2d Class Hirahie and persistentAttributes</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>setBackgroundColor is missing</t>
+  </si>
+  <si>
+    <t>Other important Methods</t>
+  </si>
+  <si>
+    <t>attachResizeListener</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +418,7 @@
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -423,20 +429,23 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -446,13 +455,16 @@
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -460,7 +472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>

</xml_diff>